<commit_message>
finish final assembly for rendering
</commit_message>
<xml_diff>
--- a/Hardware/slip_ring_wiring.xlsx
+++ b/Hardware/slip_ring_wiring.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charles\Documents\Projects\Lyra (ME102B Project)\Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{879711EA-1CDE-41CF-8772-29FD0EF9D5DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E554077-F13B-4429-BBB7-A51D24DC6F15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38295" yWindow="8865" windowWidth="21810" windowHeight="18945" xr2:uid="{FE82410B-74E8-4A93-BB81-A19E47581DEA}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="23595" windowHeight="20985" xr2:uid="{FE82410B-74E8-4A93-BB81-A19E47581DEA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="33">
   <si>
     <t>Black</t>
   </si>
@@ -83,9 +83,6 @@
     <t>Dark Brown</t>
   </si>
   <si>
-    <t>Signal</t>
-  </si>
-  <si>
     <t>Mot 2 DIR</t>
   </si>
   <si>
@@ -132,6 +129,12 @@
   </si>
   <si>
     <t>24V</t>
+  </si>
+  <si>
+    <t>Base Signal</t>
+  </si>
+  <si>
+    <t>Joint 4 Signal</t>
   </si>
 </sst>
 </file>
@@ -512,18 +515,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5282BB6D-1564-49C7-9156-5F4BA4AC6DFD}">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -531,10 +535,14 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="1"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -542,10 +550,13 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="D2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -553,10 +564,13 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="D3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -564,10 +578,13 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="D4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -575,34 +592,46 @@
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="D5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="D6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="D7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="D8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -610,18 +639,24 @@
         <v>4</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="D9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="D10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -629,26 +664,35 @@
         <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="D11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="D12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>4</v>
       </c>
       <c r="C13" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="D13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -656,10 +700,13 @@
         <v>11</v>
       </c>
       <c r="C14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="D14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>4</v>
       </c>
@@ -667,10 +714,13 @@
         <v>12</v>
       </c>
       <c r="C15" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="D15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -678,10 +728,13 @@
         <v>6</v>
       </c>
       <c r="C16" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="D16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -689,10 +742,13 @@
         <v>5</v>
       </c>
       <c r="C17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="D17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -700,18 +756,24 @@
         <v>7</v>
       </c>
       <c r="C18" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="D18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>13</v>
       </c>
       <c r="C19" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="D19" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>13</v>
       </c>
@@ -719,10 +781,13 @@
         <v>4</v>
       </c>
       <c r="C20" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="D20" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>13</v>
       </c>
@@ -730,39 +795,54 @@
         <v>9</v>
       </c>
       <c r="C21" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="D21" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>6</v>
       </c>
       <c r="C22" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="D22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>11</v>
       </c>
       <c r="C23" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="D23" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>5</v>
       </c>
       <c r="C24" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="D24" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>12</v>
       </c>
       <c r="C25" t="s">
-        <v>31</v>
+        <v>30</v>
+      </c>
+      <c r="D25" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>